<commit_message>
vault backup: 2024-04-15 08:05:42
</commit_message>
<xml_diff>
--- a/projects/quote-process-optimization/cwsell-quote-matrix.xlsx
+++ b/projects/quote-process-optimization/cwsell-quote-matrix.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://meriplex-my.sharepoint.com/personal/ian_wheeler_meriplex_com/Documents/Documents/Obsidian/Meriplex/projects/quote-process-optimization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{717D1C2B-BBD1-4E0F-B6B5-B197DFF57220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="124" documentId="8_{717D1C2B-BBD1-4E0F-B6B5-B197DFF57220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72F95B9E-431C-479E-934D-CA09B98940BE}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="13896" firstSheet="1" activeTab="4" xr2:uid="{6D55FE8F-C9AB-43F7-9348-63EA4D2256B3}"/>
+    <workbookView xWindow="28680" yWindow="450" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{6D55FE8F-C9AB-43F7-9348-63EA4D2256B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Quote Setup Field Desc." sheetId="1" r:id="rId1"/>
-    <sheet name="Quote Management Field Desc." sheetId="2" r:id="rId2"/>
-    <sheet name="Security Field Desc." sheetId="3" r:id="rId3"/>
-    <sheet name="Display Field Desc." sheetId="4" r:id="rId4"/>
-    <sheet name="Manager Approvals Field Desc." sheetId="5" r:id="rId5"/>
+    <sheet name="Quote Templates" sheetId="6" r:id="rId2"/>
+    <sheet name="Quote Management Field Desc." sheetId="2" r:id="rId3"/>
+    <sheet name="Security Field Desc." sheetId="3" r:id="rId4"/>
+    <sheet name="Display Field Desc." sheetId="4" r:id="rId5"/>
+    <sheet name="Manager Approvals Field Desc." sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="218">
   <si>
     <t>Field</t>
   </si>
@@ -212,13 +213,499 @@
   </si>
   <si>
     <t>Items with a zero cost will not be calculated into the quote margin calculation.</t>
+  </si>
+  <si>
+    <t>Quote Template Name</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>AM - Block of Hours - Blended Rates</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>AM - NRR</t>
+  </si>
+  <si>
+    <t>Training/descriptive template</t>
+  </si>
+  <si>
+    <t>AM - Time and Materials (TnM) - STD</t>
+  </si>
+  <si>
+    <t>Annual NRR Upfront Pay</t>
+  </si>
+  <si>
+    <t>Change Order</t>
+  </si>
+  <si>
+    <t>F1 GCC High Licenses - Add On Orders</t>
+  </si>
+  <si>
+    <t>F1 GCC High Licenses / Contract - Addendum</t>
+  </si>
+  <si>
+    <t>F1 Project - Fixed Price</t>
+  </si>
+  <si>
+    <t>F1 Project - Fixed Price - Bronze</t>
+  </si>
+  <si>
+    <t>F1 Project - Fixed Price - Pre 2024 Gold/Silver/Hybrid</t>
+  </si>
+  <si>
+    <t>F1 Project - Time &amp; Materials</t>
+  </si>
+  <si>
+    <t>F1 Project - Time &amp; Materials - Bronze</t>
+  </si>
+  <si>
+    <t>Government - Block of Hours - Actual Rates</t>
+  </si>
+  <si>
+    <t>Government - Block of Hours - Blended Rates</t>
+  </si>
+  <si>
+    <t>Government - Non-Recurring</t>
+  </si>
+  <si>
+    <t>Government - Non-Recurring (Legacy Bronze)</t>
+  </si>
+  <si>
+    <t>Government - Renewal</t>
+  </si>
+  <si>
+    <t>HPE Warranty Renewals</t>
+  </si>
+  <si>
+    <t>Network Infrastructure and Security Assessment Template - Paul Wartenberg</t>
+  </si>
+  <si>
+    <t>Nimble Storage Support Renewal -1 Year</t>
+  </si>
+  <si>
+    <t>Non-Recurring</t>
+  </si>
+  <si>
+    <t>NRR - Communications - Cabling - NEW</t>
+  </si>
+  <si>
+    <t>OHD Master Quotes</t>
+  </si>
+  <si>
+    <t>Physical Security - NRR</t>
+  </si>
+  <si>
+    <t>Project to Replace Existing Firewall which is going End Of Service</t>
+  </si>
+  <si>
+    <t>PSEC - Physical Security</t>
+  </si>
+  <si>
+    <t>Renewal</t>
+  </si>
+  <si>
+    <t>Security Risk Assessment</t>
+  </si>
+  <si>
+    <t>VMS NRR - Fixed Labor Rates</t>
+  </si>
+  <si>
+    <t>VMS NRR - PSP Labor Rates</t>
+  </si>
+  <si>
+    <t>VMS Renewals</t>
+  </si>
+  <si>
+    <t>1 Year MRR Subscription</t>
+  </si>
+  <si>
+    <t>AM - Block of Hours - Actual Rates</t>
+  </si>
+  <si>
+    <t>AM - ESTIMATE</t>
+  </si>
+  <si>
+    <t>AM - Meriplex - MRR</t>
+  </si>
+  <si>
+    <t>AM - Meriplex - MRR Cloud</t>
+  </si>
+  <si>
+    <t>Annual Upfront Pay - ARR</t>
+  </si>
+  <si>
+    <t>Avita - New Site</t>
+  </si>
+  <si>
+    <t>Backup of AM - Microsoft 365 MASTER Agreement Additions</t>
+  </si>
+  <si>
+    <t>Basic HW/SW Template</t>
+  </si>
+  <si>
+    <t>Basic Quote Template</t>
+  </si>
+  <si>
+    <t>BB and SDWan</t>
+  </si>
+  <si>
+    <t>Bluebeam License Subscription Addition</t>
+  </si>
+  <si>
+    <t>Communications - SCI - IPT/Wireless/Switching</t>
+  </si>
+  <si>
+    <t>Communications - Site Assessment</t>
+  </si>
+  <si>
+    <t>Communications Additions/Addendum</t>
+  </si>
+  <si>
+    <t>CPI - Products &amp; Services Master v3</t>
+  </si>
+  <si>
+    <t>CPI- NetManage and NetSecure - 2022</t>
+  </si>
+  <si>
+    <t>Cyberian Managed Services Agreement</t>
+  </si>
+  <si>
+    <t>Datto S4 Business Continuity and Disaster Recovery (BCDR) Solution</t>
+  </si>
+  <si>
+    <t>Datto S5 Business Continuity and Disaster Recovery (BCDR) Solution</t>
+  </si>
+  <si>
+    <t>Detailed HW/SW Template</t>
+  </si>
+  <si>
+    <t>Dial2Teams Template</t>
+  </si>
+  <si>
+    <t>DO NOT USE - Government M365 GCC High</t>
+  </si>
+  <si>
+    <t>Do Not Use - Meriplex Tab Templates</t>
+  </si>
+  <si>
+    <t>DO NOT USE Government - MSP A LA Cart 2.0</t>
+  </si>
+  <si>
+    <t>DO NOT USE YET - Term Options</t>
+  </si>
+  <si>
+    <t>ESTIMATE</t>
+  </si>
+  <si>
+    <t>F1 Microsoft 365 NCE Subscription</t>
+  </si>
+  <si>
+    <t>Government - Meriplex Managed Microsoft M365+ Service (Commercial/Non-Profit)</t>
+  </si>
+  <si>
+    <t>Government - MRR - Change Order (CO)/Amendment/Renewal</t>
+  </si>
+  <si>
+    <t>Government MRR - STD</t>
+  </si>
+  <si>
+    <t>IaaS / DRaaS</t>
+  </si>
+  <si>
+    <t>IMO - White Label MSP Services</t>
+  </si>
+  <si>
+    <t>IMO-White Label MSP Services</t>
+  </si>
+  <si>
+    <t>John - PC</t>
+  </si>
+  <si>
+    <t>John - Shipping Costs</t>
+  </si>
+  <si>
+    <t>M365 - Annual Recurring</t>
+  </si>
+  <si>
+    <t>MCS3</t>
+  </si>
+  <si>
+    <t>MCS3 - Amendment</t>
+  </si>
+  <si>
+    <t>Meriplex - MRR - Change Order (CO)/Amendment/Renewal</t>
+  </si>
+  <si>
+    <t>Meriplex Internal</t>
+  </si>
+  <si>
+    <t>Meriplex Managed Microsoft M365+ Service</t>
+  </si>
+  <si>
+    <t>Meriplex MSSP - Managed SIEM with Platinum Endpoint Protection</t>
+  </si>
+  <si>
+    <t>Microsoft 365 License Election - Acquisition Version</t>
+  </si>
+  <si>
+    <t>Microsoft 365 MASTER Agreement</t>
+  </si>
+  <si>
+    <t>Microsoft Copilot for Microsoft 365</t>
+  </si>
+  <si>
+    <t>Microsoft MASTER Agreement Addition(s)</t>
+  </si>
+  <si>
+    <t>Microsoft Master Agreement Additions</t>
+  </si>
+  <si>
+    <t>Microsoft NCE Election Agreement</t>
+  </si>
+  <si>
+    <t>MRR - STD</t>
+  </si>
+  <si>
+    <t>MRR - STD - Version 2</t>
+  </si>
+  <si>
+    <t>MSP 2024</t>
+  </si>
+  <si>
+    <t>MSP -A LA Cart 2.0</t>
+  </si>
+  <si>
+    <t>MSP Input Template 2022</t>
+  </si>
+  <si>
+    <t>MSP Input Template 2023</t>
+  </si>
+  <si>
+    <t>MSP Test</t>
+  </si>
+  <si>
+    <t>New Microsoft Master Agreement</t>
+  </si>
+  <si>
+    <t>Next Gen Cloud</t>
+  </si>
+  <si>
+    <t>Next Gen Cyber Security Suite</t>
+  </si>
+  <si>
+    <t>Next Gen Managed IT</t>
+  </si>
+  <si>
+    <t>Northstar-MMRC- MSP &amp; MSSP</t>
+  </si>
+  <si>
+    <t>ONI - Basic Quote Template</t>
+  </si>
+  <si>
+    <t>Per Service Ticket # 10549505 - Standard SSL Certificate For classicbevco.com</t>
+  </si>
+  <si>
+    <t>Per Service Ticket # 117342 - Zix Renewal - Annual Subscription</t>
+  </si>
+  <si>
+    <t>Plan Comparison Input 2023</t>
+  </si>
+  <si>
+    <t>Project with Phases Converted</t>
+  </si>
+  <si>
+    <t>Recurring Block - Dollars per Month - Actual Labor Rates</t>
+  </si>
+  <si>
+    <t>Recurring Block - Hours Per Month - Blended Labor Rates</t>
+  </si>
+  <si>
+    <t>Reliable IT (RIT) IT/SRA Security Risk Assessment Template</t>
+  </si>
+  <si>
+    <t>SCI - MRR</t>
+  </si>
+  <si>
+    <t>Service Cancellation Letter</t>
+  </si>
+  <si>
+    <t>Solutions - Reorder MASTER TEMPLATE</t>
+  </si>
+  <si>
+    <t>System Template - Do Not Use - MSP Plan Comparison Layout</t>
+  </si>
+  <si>
+    <t>Test Template Order Porter Name</t>
+  </si>
+  <si>
+    <t>TrustX Staff Augmentation</t>
+  </si>
+  <si>
+    <t>UCaaS</t>
+  </si>
+  <si>
+    <t>UCaaS Contract Replacement MTM</t>
+  </si>
+  <si>
+    <t>Upgrade 510s to 620s - 3 sites</t>
+  </si>
+  <si>
+    <t>VMS MRR - Fixed Labor Rates</t>
+  </si>
+  <si>
+    <t>VMS MRR - PSP Labor Rates</t>
+  </si>
+  <si>
+    <t>VMS Tab Template (Do Not Use or Delete)</t>
+  </si>
+  <si>
+    <t>Brian McShane</t>
+  </si>
+  <si>
+    <t>Cynthia Newsom</t>
+  </si>
+  <si>
+    <t>Jackie Moore</t>
+  </si>
+  <si>
+    <t>Jerry Prestridge</t>
+  </si>
+  <si>
+    <t>John Sobernheim</t>
+  </si>
+  <si>
+    <t>Laura Emery</t>
+  </si>
+  <si>
+    <t>Michael True</t>
+  </si>
+  <si>
+    <t>Ron Walker</t>
+  </si>
+  <si>
+    <t>Shaun Kilkenny</t>
+  </si>
+  <si>
+    <t>Anthony Kazlauskas</t>
+  </si>
+  <si>
+    <t>We use this for NRR Annual upfront pay for Microsoft 365, EP</t>
+  </si>
+  <si>
+    <t>Keep</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>New Quote Template Name</t>
+  </si>
+  <si>
+    <t>MPC-NRR-AM</t>
+  </si>
+  <si>
+    <t>MPC-HYBRID-AM-BOH-BlendedRates</t>
+  </si>
+  <si>
+    <t>MPC-HYBRID-AM-TNM-STD</t>
+  </si>
+  <si>
+    <t>MPC-NRR-Annual-UpfrontPay</t>
+  </si>
+  <si>
+    <t>MPC-HYBRID-ChangeOrder</t>
+  </si>
+  <si>
+    <t>F1-NRR-GCCHigh-AddOnOrders</t>
+  </si>
+  <si>
+    <t>F1-NRR-GCCHigh-Addendum</t>
+  </si>
+  <si>
+    <t>F1-NRR-Project-FixedPrice</t>
+  </si>
+  <si>
+    <t>F1-NRR-Project-FixedPrice-Bronze</t>
+  </si>
+  <si>
+    <t>F1-HYBRID-Project-FixedPrice-Pre2024-GoldSilverHybrid</t>
+  </si>
+  <si>
+    <t>F1-NRR-Project-TimeAndMaterials</t>
+  </si>
+  <si>
+    <t>F1-NRR-Project-TimeAndMaterials-Bronze</t>
+  </si>
+  <si>
+    <t>MPC-HYBRID-GOV-BOH-ActualRates</t>
+  </si>
+  <si>
+    <t>MPC-HYBRID-GOV-BOH-BlendedRates</t>
+  </si>
+  <si>
+    <t>MPC-NRR-GOV</t>
+  </si>
+  <si>
+    <t>MPC-NRR-GOV-LegacyBronze</t>
+  </si>
+  <si>
+    <t>MPC-MRR-GOV-Renewal</t>
+  </si>
+  <si>
+    <t>MPC-MRR-HPE-WarrantyRenewals</t>
+  </si>
+  <si>
+    <t>MPC-NRR-NetworkInfrastructureSecurityAssessment-PaulWartenberg</t>
+  </si>
+  <si>
+    <t>MPC-MRR-NimbleStorage-SupportRenewal-1Year</t>
+  </si>
+  <si>
+    <t>MPC-NRR-Communications-Cabling-NEW</t>
+  </si>
+  <si>
+    <t>MPC-HYBRID-OHD-MasterQuotes</t>
+  </si>
+  <si>
+    <t>MPC-NRR-PhysicalSecurity</t>
+  </si>
+  <si>
+    <t>MPC-NRR-Project-ReplaceFirewall-EndOfService</t>
+  </si>
+  <si>
+    <t>MPC-MRR-PSEC-PhysicalSecurity-Renewal</t>
+  </si>
+  <si>
+    <t>MPC-NRR-SecurityRiskAssessment</t>
+  </si>
+  <si>
+    <t>VMS-NRR-FixedLaborRates</t>
+  </si>
+  <si>
+    <t>VMS-NRR-PSPLaborRates</t>
+  </si>
+  <si>
+    <t>VMS-MRR-Renewals</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,8 +736,30 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -269,8 +778,25 @@
         <bgColor theme="0" tint="-0.34998626667073579"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -293,12 +819,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -311,22 +849,106 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="1" builtinId="15"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="34">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -384,13 +1006,38 @@
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Display"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -409,55 +1056,84 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B7E9B8F6-B0E1-4B46-9D20-BCF51735F1A3}" name="Table1" displayName="Table1" ref="A1:B8" totalsRowShown="0" dataDxfId="15" headerRowCellStyle="Title">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B7E9B8F6-B0E1-4B46-9D20-BCF51735F1A3}" name="Table1" displayName="Table1" ref="A1:B8" totalsRowShown="0" dataDxfId="33" headerRowCellStyle="Title">
   <autoFilter ref="A1:B8" xr:uid="{B7E9B8F6-B0E1-4B46-9D20-BCF51735F1A3}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{293AFF5D-0C58-439C-A9DA-8482E2358D97}" name="Field" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{7769824F-C699-45D6-AF6E-03B2011102B1}" name="Description" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{293AFF5D-0C58-439C-A9DA-8482E2358D97}" name="Field" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{7769824F-C699-45D6-AF6E-03B2011102B1}" name="Description" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium22" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{20723ADE-D95B-4E73-9206-81D1E73DB870}" name="Table14" displayName="Table14" ref="A1:B8" totalsRowShown="0" dataDxfId="12" headerRowCellStyle="Title">
-  <autoFilter ref="A1:B8" xr:uid="{20723ADE-D95B-4E73-9206-81D1E73DB870}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{42EA7B49-913E-4330-B326-AAF244926227}" name="Field" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{46545A5F-93B3-4E56-8EC1-68B0F0B3B1BD}" name="Description" dataDxfId="10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C826E71F-1F09-4E74-AB87-A4B764A79312}" name="Table4" displayName="Table4" ref="A1:Q116" totalsRowShown="0" headerRowDxfId="30">
+  <autoFilter ref="A1:Q116" xr:uid="{C826E71F-1F09-4E74-AB87-A4B764A79312}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G116">
+    <sortCondition sortBy="cellColor" ref="A1:A116" dxfId="29"/>
+  </sortState>
+  <tableColumns count="17">
+    <tableColumn id="1" xr3:uid="{1CDAD25C-2B9A-49A0-AF29-91C07A6E557F}" name="Quote Template Name"/>
+    <tableColumn id="3" xr3:uid="{5EACD7CE-28E1-4D84-9371-73FEAE60A99A}" name="New Quote Template Name"/>
+    <tableColumn id="2" xr3:uid="{34F03541-91C6-46B7-85FD-240B5B3CA00D}" name="Number" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{B8CFDEBF-A2AA-4EC4-8AE2-7AA874916A15}" name="Status" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{BA7416B4-3F5E-40EA-AD3C-257EA87B11DA}" name="Description"/>
+    <tableColumn id="7" xr3:uid="{78D4773A-F41A-4332-990A-390F054BF842}" name="Action" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{3E2DAFC4-4656-494A-8EBC-191A5A3B8CD9}" name="Notes"/>
+    <tableColumn id="9" xr3:uid="{92747196-C02D-44EE-A00E-88D89FCA3928}" name="Brian McShane" dataDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{11D5791E-3C3C-4638-8988-3326D72C0B2F}" name="Cynthia Newsom" dataDxfId="13"/>
+    <tableColumn id="11" xr3:uid="{D425B706-2CE8-49E4-B19D-803E5519746B}" name="Jackie Moore" dataDxfId="12"/>
+    <tableColumn id="12" xr3:uid="{1A6DBD9C-5080-4FDB-AC9D-378744BB47DF}" name="Jerry Prestridge" dataDxfId="11"/>
+    <tableColumn id="13" xr3:uid="{917A0CCE-95BA-4484-B3CA-99D29C5F0E5D}" name="John Sobernheim" dataDxfId="10"/>
+    <tableColumn id="14" xr3:uid="{34C6A6A8-871B-46B7-8595-DD76FDE12BEA}" name="Laura Emery" dataDxfId="9"/>
+    <tableColumn id="15" xr3:uid="{02D2670E-D76F-41CF-9F8F-159FA85FEAEF}" name="Michael True" dataDxfId="8"/>
+    <tableColumn id="16" xr3:uid="{57A23E55-7D1C-45D5-8657-75F1757A1472}" name="Ron Walker" dataDxfId="7"/>
+    <tableColumn id="17" xr3:uid="{282EDB90-C5B8-4965-9660-1C5DDAC1DE61}" name="Shaun Kilkenny" dataDxfId="6"/>
+    <tableColumn id="18" xr3:uid="{E0737ADE-6ACC-4DE0-B628-AD8F31CA7CFC}" name="Anthony Kazlauskas" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium22" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{196ED135-BB9E-4142-9488-3FD586A38595}" name="Table146" displayName="Table146" ref="A1:B8" totalsRowShown="0" dataDxfId="9" headerRowCellStyle="Title">
-  <autoFilter ref="A1:B8" xr:uid="{196ED135-BB9E-4142-9488-3FD586A38595}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{20723ADE-D95B-4E73-9206-81D1E73DB870}" name="Table14" displayName="Table14" ref="A1:B8" totalsRowShown="0" dataDxfId="27" headerRowCellStyle="Title">
+  <autoFilter ref="A1:B8" xr:uid="{20723ADE-D95B-4E73-9206-81D1E73DB870}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{A2630032-F8A3-4E83-9919-5BF67C776B4F}" name="Field" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{B56F3135-55F6-4793-A7CF-20BEB6D575E1}" name="Description" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{42EA7B49-913E-4330-B326-AAF244926227}" name="Field" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{46545A5F-93B3-4E56-8EC1-68B0F0B3B1BD}" name="Description" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium22" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{19510359-701A-45C0-BDE2-B0F05B9E4D3E}" name="Table1467" displayName="Table1467" ref="A1:B5" totalsRowShown="0" dataDxfId="6" headerRowCellStyle="Title">
-  <autoFilter ref="A1:B5" xr:uid="{19510359-701A-45C0-BDE2-B0F05B9E4D3E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{196ED135-BB9E-4142-9488-3FD586A38595}" name="Table146" displayName="Table146" ref="A1:B8" totalsRowShown="0" dataDxfId="24" headerRowCellStyle="Title">
+  <autoFilter ref="A1:B8" xr:uid="{196ED135-BB9E-4142-9488-3FD586A38595}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{946DDB50-8E80-4711-8DC2-4CF620D45D3A}" name="Field" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{119F63D1-C0E3-49C5-83FA-FBC8FEAFD63A}" name="Description" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{A2630032-F8A3-4E83-9919-5BF67C776B4F}" name="Field" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{B56F3135-55F6-4793-A7CF-20BEB6D575E1}" name="Description" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium22" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{57E60675-07BB-4BC1-98E6-F1A7C439A2AE}" name="Table14679" displayName="Table14679" ref="A1:B4" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2" headerRowCellStyle="Title">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{19510359-701A-45C0-BDE2-B0F05B9E4D3E}" name="Table1467" displayName="Table1467" ref="A1:B5" totalsRowShown="0" dataDxfId="21" headerRowCellStyle="Title">
+  <autoFilter ref="A1:B5" xr:uid="{19510359-701A-45C0-BDE2-B0F05B9E4D3E}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{946DDB50-8E80-4711-8DC2-4CF620D45D3A}" name="Field" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{119F63D1-C0E3-49C5-83FA-FBC8FEAFD63A}" name="Description" dataDxfId="19"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium22" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{57E60675-07BB-4BC1-98E6-F1A7C439A2AE}" name="Table14679" displayName="Table14679" ref="A1:B4" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" headerRowCellStyle="Title">
   <autoFilter ref="A1:B4" xr:uid="{57E60675-07BB-4BC1-98E6-F1A7C439A2AE}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{8C23B5EC-197F-4876-9594-2DC49CDFE43E}" name="Field" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{DE73CB7B-12DD-4809-8421-3EE3FAAB7BCA}" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{8C23B5EC-197F-4876-9594-2DC49CDFE43E}" name="Field" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{DE73CB7B-12DD-4809-8421-3EE3FAAB7BCA}" name="Description" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium22" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -865,6 +1541,2904 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23C2E8FE-9516-4800-BF01-34B33BCED5BC}">
+  <dimension ref="A1:Q116"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="75.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="75.7109375" customWidth="1"/>
+    <col min="8" max="17" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="N1" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="O1" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="P1" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q1" s="14" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="C2" s="11">
+        <v>84520</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="10"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="C3" s="10">
+        <v>82873</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="16"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="C4" s="11">
+        <v>84521</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="C5" s="11">
+        <v>125547</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="K5" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="C6" s="11">
+        <v>5250</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="K6" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="L6" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q6" s="16" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="C7" s="11">
+        <v>123332</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="C8" s="11">
+        <v>123330</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="C9" s="11">
+        <v>123316</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="N9" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="C10" s="11">
+        <v>123338</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="N10" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="C11" s="11">
+        <v>123339</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="N11" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="C12" s="11">
+        <v>123328</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="N12" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="C13" s="11">
+        <v>123340</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="N13" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="16"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="C14" s="11">
+        <v>125560</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="10"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="M14" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="16"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="C15" s="11">
+        <v>125561</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="10"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="M15" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="16"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="C16" s="11">
+        <v>125439</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="M16" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="C17" s="11">
+        <v>125474</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="M17" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="N17" s="16"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="C18" s="11">
+        <v>125512</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="10"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="N18" s="16"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="16"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="C19" s="11">
+        <v>113536</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="16"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="C20" s="11">
+        <v>123211</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" s="10"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="16"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="C21" s="11">
+        <v>112657</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" s="10"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="16"/>
+      <c r="P21" s="16"/>
+      <c r="Q21" s="16"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" s="10"/>
+      <c r="C22" s="11">
+        <v>107946</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" s="10"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="K22" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="L22" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="M22" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="N22" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="O22" s="16"/>
+      <c r="P22" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q22" s="16" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="C23" s="11">
+        <v>83706</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="O23" s="16"/>
+      <c r="P23" s="16"/>
+      <c r="Q23" s="16"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="C24" s="11">
+        <v>110471</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="10"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="O24" s="16"/>
+      <c r="P24" s="16"/>
+      <c r="Q24" s="16"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="C25" s="11">
+        <v>111328</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25" s="10"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="O25" s="16"/>
+      <c r="P25" s="16"/>
+      <c r="Q25" s="16"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="C26" s="11">
+        <v>115720</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" s="10"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="M26" s="16"/>
+      <c r="N26" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="O26" s="16"/>
+      <c r="P26" s="16"/>
+      <c r="Q26" s="16"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C27" s="11">
+        <v>104974</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E27" s="10"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="16"/>
+      <c r="Q27" s="16"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B28" s="10"/>
+      <c r="C28" s="11">
+        <v>111302</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E28" s="10"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="K28" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="L28" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="M28" s="16"/>
+      <c r="N28" s="16"/>
+      <c r="O28" s="16"/>
+      <c r="P28" s="16"/>
+      <c r="Q28" s="16"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="C29" s="11">
+        <v>124711</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E29" s="10"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="16"/>
+      <c r="L29" s="16"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="O29" s="16"/>
+      <c r="P29" s="16"/>
+      <c r="Q29" s="16"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="C30" s="11">
+        <v>120881</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" s="10"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="16"/>
+      <c r="L30" s="16"/>
+      <c r="M30" s="16"/>
+      <c r="N30" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="O30" s="16"/>
+      <c r="P30" s="16"/>
+      <c r="Q30" s="16"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="C31" s="11">
+        <v>120885</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E31" s="10"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="16"/>
+      <c r="M31" s="16"/>
+      <c r="N31" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="O31" s="16"/>
+      <c r="P31" s="16"/>
+      <c r="Q31" s="16"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="C32" s="11">
+        <v>120883</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E32" s="10"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="16"/>
+      <c r="K32" s="16"/>
+      <c r="L32" s="16"/>
+      <c r="M32" s="16"/>
+      <c r="N32" s="16"/>
+      <c r="O32" s="16"/>
+      <c r="P32" s="16"/>
+      <c r="Q32" s="16"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" s="12">
+        <v>117939</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F33" s="18"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="18"/>
+      <c r="J33" s="18"/>
+      <c r="K33" s="18"/>
+      <c r="L33" s="18"/>
+      <c r="M33" s="18"/>
+      <c r="N33" s="18"/>
+      <c r="O33" s="18"/>
+      <c r="P33" s="18"/>
+      <c r="Q33" s="18"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>95</v>
+      </c>
+      <c r="C34" s="12">
+        <v>121097</v>
+      </c>
+      <c r="D34" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="18"/>
+      <c r="M34" s="18"/>
+      <c r="N34" s="18"/>
+      <c r="O34" s="18"/>
+      <c r="P34" s="18"/>
+      <c r="Q34" s="18"/>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>96</v>
+      </c>
+      <c r="C35" s="12">
+        <v>106952</v>
+      </c>
+      <c r="D35" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F35" s="18"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="18"/>
+      <c r="L35" s="18"/>
+      <c r="M35" s="18"/>
+      <c r="N35" s="18"/>
+      <c r="O35" s="18"/>
+      <c r="P35" s="18"/>
+      <c r="Q35" s="18"/>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>97</v>
+      </c>
+      <c r="C36" s="12">
+        <v>79365</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="18"/>
+      <c r="M36" s="18"/>
+      <c r="N36" s="18"/>
+      <c r="O36" s="18"/>
+      <c r="P36" s="18"/>
+      <c r="Q36" s="18"/>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>98</v>
+      </c>
+      <c r="C37" s="12">
+        <v>80457</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F37" s="18"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="18"/>
+      <c r="J37" s="18"/>
+      <c r="K37" s="18"/>
+      <c r="L37" s="18"/>
+      <c r="M37" s="18"/>
+      <c r="N37" s="18"/>
+      <c r="O37" s="18"/>
+      <c r="P37" s="18"/>
+      <c r="Q37" s="18"/>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>99</v>
+      </c>
+      <c r="C38" s="12">
+        <v>113160</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F38" s="18"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="18"/>
+      <c r="J38" s="18"/>
+      <c r="K38" s="18"/>
+      <c r="L38" s="18"/>
+      <c r="M38" s="18"/>
+      <c r="N38" s="18"/>
+      <c r="O38" s="18"/>
+      <c r="P38" s="18"/>
+      <c r="Q38" s="18"/>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>100</v>
+      </c>
+      <c r="C39" s="12">
+        <v>95881</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F39" s="18"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="18"/>
+      <c r="J39" s="18"/>
+      <c r="K39" s="18"/>
+      <c r="L39" s="18"/>
+      <c r="M39" s="18"/>
+      <c r="N39" s="18"/>
+      <c r="O39" s="18"/>
+      <c r="P39" s="18"/>
+      <c r="Q39" s="18"/>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>101</v>
+      </c>
+      <c r="C40" s="12">
+        <v>112518</v>
+      </c>
+      <c r="D40" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F40" s="18"/>
+      <c r="H40" s="18"/>
+      <c r="I40" s="18"/>
+      <c r="J40" s="18"/>
+      <c r="K40" s="18"/>
+      <c r="L40" s="18"/>
+      <c r="M40" s="18"/>
+      <c r="N40" s="18"/>
+      <c r="O40" s="18"/>
+      <c r="P40" s="18"/>
+      <c r="Q40" s="18"/>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>102</v>
+      </c>
+      <c r="C41" s="12">
+        <v>117829</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F41" s="18"/>
+      <c r="H41" s="18"/>
+      <c r="I41" s="18"/>
+      <c r="J41" s="18"/>
+      <c r="K41" s="18"/>
+      <c r="L41" s="18"/>
+      <c r="M41" s="18"/>
+      <c r="N41" s="18"/>
+      <c r="O41" s="18"/>
+      <c r="P41" s="18"/>
+      <c r="Q41" s="18"/>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>103</v>
+      </c>
+      <c r="C42" s="12">
+        <v>117831</v>
+      </c>
+      <c r="D42" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F42" s="18"/>
+      <c r="H42" s="18"/>
+      <c r="I42" s="18"/>
+      <c r="J42" s="18"/>
+      <c r="K42" s="18"/>
+      <c r="L42" s="18"/>
+      <c r="M42" s="18"/>
+      <c r="N42" s="18"/>
+      <c r="O42" s="18"/>
+      <c r="P42" s="18"/>
+      <c r="Q42" s="18"/>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>104</v>
+      </c>
+      <c r="C43" s="12">
+        <v>114792</v>
+      </c>
+      <c r="D43" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F43" s="18"/>
+      <c r="H43" s="18"/>
+      <c r="I43" s="18"/>
+      <c r="J43" s="18"/>
+      <c r="K43" s="18"/>
+      <c r="L43" s="18"/>
+      <c r="M43" s="18"/>
+      <c r="N43" s="18"/>
+      <c r="O43" s="18"/>
+      <c r="P43" s="18"/>
+      <c r="Q43" s="18"/>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>105</v>
+      </c>
+      <c r="C44" s="12">
+        <v>116542</v>
+      </c>
+      <c r="D44" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F44" s="18"/>
+      <c r="H44" s="18"/>
+      <c r="I44" s="18"/>
+      <c r="J44" s="18"/>
+      <c r="K44" s="18"/>
+      <c r="L44" s="18"/>
+      <c r="M44" s="18"/>
+      <c r="N44" s="18"/>
+      <c r="O44" s="18"/>
+      <c r="P44" s="18"/>
+      <c r="Q44" s="18"/>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>106</v>
+      </c>
+      <c r="C45" s="12">
+        <v>5255</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F45" s="18"/>
+      <c r="H45" s="18"/>
+      <c r="I45" s="18"/>
+      <c r="J45" s="18"/>
+      <c r="K45" s="18"/>
+      <c r="L45" s="18"/>
+      <c r="M45" s="18"/>
+      <c r="N45" s="18"/>
+      <c r="O45" s="18"/>
+      <c r="P45" s="18"/>
+      <c r="Q45" s="18"/>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>107</v>
+      </c>
+      <c r="C46" s="12">
+        <v>5706</v>
+      </c>
+      <c r="D46" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F46" s="18"/>
+      <c r="H46" s="18"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
+      <c r="K46" s="18"/>
+      <c r="L46" s="18"/>
+      <c r="M46" s="18"/>
+      <c r="N46" s="18"/>
+      <c r="O46" s="18"/>
+      <c r="P46" s="18"/>
+      <c r="Q46" s="18"/>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>108</v>
+      </c>
+      <c r="C47" s="12">
+        <v>114563</v>
+      </c>
+      <c r="D47" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F47" s="18"/>
+      <c r="H47" s="18"/>
+      <c r="I47" s="18"/>
+      <c r="J47" s="18"/>
+      <c r="K47" s="18"/>
+      <c r="L47" s="18"/>
+      <c r="M47" s="18"/>
+      <c r="N47" s="18"/>
+      <c r="O47" s="18"/>
+      <c r="P47" s="18"/>
+      <c r="Q47" s="18"/>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>109</v>
+      </c>
+      <c r="C48" s="12">
+        <v>120261</v>
+      </c>
+      <c r="D48" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F48" s="18"/>
+      <c r="H48" s="18"/>
+      <c r="I48" s="18"/>
+      <c r="J48" s="18"/>
+      <c r="K48" s="18"/>
+      <c r="L48" s="18"/>
+      <c r="M48" s="18"/>
+      <c r="N48" s="18"/>
+      <c r="O48" s="18"/>
+      <c r="P48" s="18"/>
+      <c r="Q48" s="18"/>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>110</v>
+      </c>
+      <c r="C49" s="12">
+        <v>120264</v>
+      </c>
+      <c r="D49" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F49" s="18"/>
+      <c r="H49" s="18"/>
+      <c r="I49" s="18"/>
+      <c r="J49" s="18"/>
+      <c r="K49" s="18"/>
+      <c r="L49" s="18"/>
+      <c r="M49" s="18"/>
+      <c r="N49" s="18"/>
+      <c r="O49" s="18"/>
+      <c r="P49" s="18"/>
+      <c r="Q49" s="18"/>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>111</v>
+      </c>
+      <c r="C50" s="12">
+        <v>118533</v>
+      </c>
+      <c r="D50" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F50" s="18"/>
+      <c r="H50" s="18"/>
+      <c r="I50" s="18"/>
+      <c r="J50" s="18"/>
+      <c r="K50" s="18"/>
+      <c r="L50" s="18"/>
+      <c r="M50" s="18"/>
+      <c r="N50" s="18"/>
+      <c r="O50" s="18"/>
+      <c r="P50" s="18"/>
+      <c r="Q50" s="18"/>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>112</v>
+      </c>
+      <c r="C51" s="12">
+        <v>110119</v>
+      </c>
+      <c r="D51" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F51" s="18"/>
+      <c r="H51" s="18"/>
+      <c r="I51" s="18"/>
+      <c r="J51" s="18"/>
+      <c r="K51" s="18"/>
+      <c r="L51" s="18"/>
+      <c r="M51" s="18"/>
+      <c r="N51" s="18"/>
+      <c r="O51" s="18"/>
+      <c r="P51" s="18"/>
+      <c r="Q51" s="18"/>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>113</v>
+      </c>
+      <c r="C52" s="12">
+        <v>117897</v>
+      </c>
+      <c r="D52" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F52" s="18"/>
+      <c r="H52" s="18"/>
+      <c r="I52" s="18"/>
+      <c r="J52" s="18"/>
+      <c r="K52" s="18"/>
+      <c r="L52" s="18"/>
+      <c r="M52" s="18"/>
+      <c r="N52" s="18"/>
+      <c r="O52" s="18"/>
+      <c r="P52" s="18"/>
+      <c r="Q52" s="18"/>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>114</v>
+      </c>
+      <c r="C53" s="12">
+        <v>117830</v>
+      </c>
+      <c r="D53" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F53" s="18"/>
+      <c r="H53" s="18"/>
+      <c r="I53" s="18"/>
+      <c r="J53" s="18"/>
+      <c r="K53" s="18"/>
+      <c r="L53" s="18"/>
+      <c r="M53" s="18"/>
+      <c r="N53" s="18"/>
+      <c r="O53" s="18"/>
+      <c r="P53" s="18"/>
+      <c r="Q53" s="18"/>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>115</v>
+      </c>
+      <c r="C54" s="12">
+        <v>118531</v>
+      </c>
+      <c r="D54" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F54" s="18"/>
+      <c r="H54" s="18"/>
+      <c r="I54" s="18"/>
+      <c r="J54" s="18"/>
+      <c r="K54" s="18"/>
+      <c r="L54" s="18"/>
+      <c r="M54" s="18"/>
+      <c r="N54" s="18"/>
+      <c r="O54" s="18"/>
+      <c r="P54" s="18"/>
+      <c r="Q54" s="18"/>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>116</v>
+      </c>
+      <c r="C55" s="12">
+        <v>125618</v>
+      </c>
+      <c r="D55" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F55" s="18"/>
+      <c r="H55" s="18"/>
+      <c r="I55" s="18"/>
+      <c r="J55" s="18"/>
+      <c r="K55" s="18"/>
+      <c r="L55" s="18"/>
+      <c r="M55" s="18"/>
+      <c r="N55" s="18"/>
+      <c r="O55" s="18"/>
+      <c r="P55" s="18"/>
+      <c r="Q55" s="18"/>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>117</v>
+      </c>
+      <c r="C56" s="12">
+        <v>111307</v>
+      </c>
+      <c r="D56" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F56" s="18"/>
+      <c r="H56" s="18"/>
+      <c r="I56" s="18"/>
+      <c r="J56" s="18"/>
+      <c r="K56" s="18"/>
+      <c r="L56" s="18"/>
+      <c r="M56" s="18"/>
+      <c r="N56" s="18"/>
+      <c r="O56" s="18"/>
+      <c r="P56" s="18"/>
+      <c r="Q56" s="18"/>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>118</v>
+      </c>
+      <c r="C57" s="12">
+        <v>125558</v>
+      </c>
+      <c r="D57" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F57" s="18"/>
+      <c r="H57" s="18"/>
+      <c r="I57" s="18"/>
+      <c r="J57" s="18"/>
+      <c r="K57" s="18"/>
+      <c r="L57" s="18"/>
+      <c r="M57" s="18"/>
+      <c r="N57" s="18"/>
+      <c r="O57" s="18"/>
+      <c r="P57" s="18"/>
+      <c r="Q57" s="18"/>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>119</v>
+      </c>
+      <c r="C58" s="12">
+        <v>116959</v>
+      </c>
+      <c r="D58" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F58" s="18"/>
+      <c r="H58" s="18"/>
+      <c r="I58" s="18"/>
+      <c r="J58" s="18"/>
+      <c r="K58" s="18"/>
+      <c r="L58" s="18"/>
+      <c r="M58" s="18"/>
+      <c r="N58" s="18"/>
+      <c r="O58" s="18"/>
+      <c r="P58" s="18"/>
+      <c r="Q58" s="18"/>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>120</v>
+      </c>
+      <c r="C59" s="12">
+        <v>112915</v>
+      </c>
+      <c r="D59" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F59" s="18"/>
+      <c r="H59" s="18"/>
+      <c r="I59" s="18"/>
+      <c r="J59" s="18"/>
+      <c r="K59" s="18"/>
+      <c r="L59" s="18"/>
+      <c r="M59" s="18"/>
+      <c r="N59" s="18"/>
+      <c r="O59" s="18"/>
+      <c r="P59" s="18"/>
+      <c r="Q59" s="18"/>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>121</v>
+      </c>
+      <c r="C60" s="12">
+        <v>123315</v>
+      </c>
+      <c r="D60" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F60" s="18"/>
+      <c r="H60" s="18"/>
+      <c r="I60" s="18"/>
+      <c r="J60" s="18"/>
+      <c r="K60" s="18"/>
+      <c r="L60" s="18"/>
+      <c r="M60" s="18"/>
+      <c r="N60" s="18"/>
+      <c r="O60" s="18"/>
+      <c r="P60" s="18"/>
+      <c r="Q60" s="18"/>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>122</v>
+      </c>
+      <c r="C61" s="12">
+        <v>125606</v>
+      </c>
+      <c r="D61" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F61" s="18"/>
+      <c r="H61" s="18"/>
+      <c r="I61" s="18"/>
+      <c r="J61" s="18"/>
+      <c r="K61" s="18"/>
+      <c r="L61" s="18"/>
+      <c r="M61" s="18"/>
+      <c r="N61" s="18"/>
+      <c r="O61" s="18"/>
+      <c r="P61" s="18"/>
+      <c r="Q61" s="18"/>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>123</v>
+      </c>
+      <c r="C62" s="12">
+        <v>125557</v>
+      </c>
+      <c r="D62" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F62" s="18"/>
+      <c r="H62" s="18"/>
+      <c r="I62" s="18"/>
+      <c r="J62" s="18"/>
+      <c r="K62" s="18"/>
+      <c r="L62" s="18"/>
+      <c r="M62" s="18"/>
+      <c r="N62" s="18"/>
+      <c r="O62" s="18"/>
+      <c r="P62" s="18"/>
+      <c r="Q62" s="18"/>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>124</v>
+      </c>
+      <c r="C63" s="12">
+        <v>125610</v>
+      </c>
+      <c r="D63" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F63" s="18"/>
+      <c r="H63" s="18"/>
+      <c r="I63" s="18"/>
+      <c r="J63" s="18"/>
+      <c r="K63" s="18"/>
+      <c r="L63" s="18"/>
+      <c r="M63" s="18"/>
+      <c r="N63" s="18"/>
+      <c r="O63" s="18"/>
+      <c r="P63" s="18"/>
+      <c r="Q63" s="18"/>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>125</v>
+      </c>
+      <c r="C64" s="12">
+        <v>107455</v>
+      </c>
+      <c r="D64" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F64" s="18"/>
+      <c r="H64" s="18"/>
+      <c r="I64" s="18"/>
+      <c r="J64" s="18"/>
+      <c r="K64" s="18"/>
+      <c r="L64" s="18"/>
+      <c r="M64" s="18"/>
+      <c r="N64" s="18"/>
+      <c r="O64" s="18"/>
+      <c r="P64" s="18"/>
+      <c r="Q64" s="18"/>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>126</v>
+      </c>
+      <c r="C65" s="12">
+        <v>107239</v>
+      </c>
+      <c r="D65" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F65" s="18"/>
+      <c r="H65" s="18"/>
+      <c r="I65" s="18"/>
+      <c r="J65" s="18"/>
+      <c r="K65" s="18"/>
+      <c r="L65" s="18"/>
+      <c r="M65" s="18"/>
+      <c r="N65" s="18"/>
+      <c r="O65" s="18"/>
+      <c r="P65" s="18"/>
+      <c r="Q65" s="18"/>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>127</v>
+      </c>
+      <c r="C66" s="12">
+        <v>107690</v>
+      </c>
+      <c r="D66" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F66" s="18"/>
+      <c r="H66" s="18"/>
+      <c r="I66" s="18"/>
+      <c r="J66" s="18"/>
+      <c r="K66" s="18"/>
+      <c r="L66" s="18"/>
+      <c r="M66" s="18"/>
+      <c r="N66" s="18"/>
+      <c r="O66" s="18"/>
+      <c r="P66" s="18"/>
+      <c r="Q66" s="18"/>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>128</v>
+      </c>
+      <c r="C67" s="12">
+        <v>122771</v>
+      </c>
+      <c r="D67" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F67" s="18"/>
+      <c r="H67" s="18"/>
+      <c r="I67" s="18"/>
+      <c r="J67" s="18"/>
+      <c r="K67" s="18"/>
+      <c r="L67" s="18"/>
+      <c r="M67" s="18"/>
+      <c r="N67" s="18"/>
+      <c r="O67" s="18"/>
+      <c r="P67" s="18"/>
+      <c r="Q67" s="18"/>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>129</v>
+      </c>
+      <c r="C68" s="12">
+        <v>124609</v>
+      </c>
+      <c r="D68" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F68" s="18"/>
+      <c r="H68" s="18"/>
+      <c r="I68" s="18"/>
+      <c r="J68" s="18"/>
+      <c r="K68" s="18"/>
+      <c r="L68" s="18"/>
+      <c r="M68" s="18"/>
+      <c r="N68" s="18"/>
+      <c r="O68" s="18"/>
+      <c r="P68" s="18"/>
+      <c r="Q68" s="18"/>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>130</v>
+      </c>
+      <c r="C69" s="12">
+        <v>116976</v>
+      </c>
+      <c r="D69" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F69" s="18"/>
+      <c r="H69" s="18"/>
+      <c r="I69" s="18"/>
+      <c r="J69" s="18"/>
+      <c r="K69" s="18"/>
+      <c r="L69" s="18"/>
+      <c r="M69" s="18"/>
+      <c r="N69" s="18"/>
+      <c r="O69" s="18"/>
+      <c r="P69" s="18"/>
+      <c r="Q69" s="18"/>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>131</v>
+      </c>
+      <c r="C70" s="12">
+        <v>5170</v>
+      </c>
+      <c r="D70" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F70" s="18"/>
+      <c r="H70" s="18"/>
+      <c r="I70" s="18"/>
+      <c r="J70" s="18"/>
+      <c r="K70" s="18"/>
+      <c r="L70" s="18"/>
+      <c r="M70" s="18"/>
+      <c r="N70" s="18"/>
+      <c r="O70" s="18"/>
+      <c r="P70" s="18"/>
+      <c r="Q70" s="18"/>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>132</v>
+      </c>
+      <c r="C71" s="12">
+        <v>78299</v>
+      </c>
+      <c r="D71" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F71" s="18"/>
+      <c r="H71" s="18"/>
+      <c r="I71" s="18"/>
+      <c r="J71" s="18"/>
+      <c r="K71" s="18"/>
+      <c r="L71" s="18"/>
+      <c r="M71" s="18"/>
+      <c r="N71" s="18"/>
+      <c r="O71" s="18"/>
+      <c r="P71" s="18"/>
+      <c r="Q71" s="18"/>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>133</v>
+      </c>
+      <c r="C72" s="12">
+        <v>78516</v>
+      </c>
+      <c r="D72" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F72" s="18"/>
+      <c r="H72" s="18"/>
+      <c r="I72" s="18"/>
+      <c r="J72" s="18"/>
+      <c r="K72" s="18"/>
+      <c r="L72" s="18"/>
+      <c r="M72" s="18"/>
+      <c r="N72" s="18"/>
+      <c r="O72" s="18"/>
+      <c r="P72" s="18"/>
+      <c r="Q72" s="18"/>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>134</v>
+      </c>
+      <c r="C73" s="12">
+        <v>95373</v>
+      </c>
+      <c r="D73" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F73" s="18"/>
+      <c r="H73" s="18"/>
+      <c r="I73" s="18"/>
+      <c r="J73" s="18"/>
+      <c r="K73" s="18"/>
+      <c r="L73" s="18"/>
+      <c r="M73" s="18"/>
+      <c r="N73" s="18"/>
+      <c r="O73" s="18"/>
+      <c r="P73" s="18"/>
+      <c r="Q73" s="18"/>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>135</v>
+      </c>
+      <c r="C74" s="12">
+        <v>112487</v>
+      </c>
+      <c r="D74" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F74" s="18"/>
+      <c r="H74" s="18"/>
+      <c r="I74" s="18"/>
+      <c r="J74" s="18"/>
+      <c r="K74" s="18"/>
+      <c r="L74" s="18"/>
+      <c r="M74" s="18"/>
+      <c r="N74" s="18"/>
+      <c r="O74" s="18"/>
+      <c r="P74" s="18"/>
+      <c r="Q74" s="18"/>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>136</v>
+      </c>
+      <c r="C75" s="12">
+        <v>113552</v>
+      </c>
+      <c r="D75" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F75" s="18"/>
+      <c r="H75" s="18"/>
+      <c r="I75" s="18"/>
+      <c r="J75" s="18"/>
+      <c r="K75" s="18"/>
+      <c r="L75" s="18"/>
+      <c r="M75" s="18"/>
+      <c r="N75" s="18"/>
+      <c r="O75" s="18"/>
+      <c r="P75" s="18"/>
+      <c r="Q75" s="18"/>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>137</v>
+      </c>
+      <c r="C76" s="12">
+        <v>108214</v>
+      </c>
+      <c r="D76" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F76" s="18"/>
+      <c r="H76" s="18"/>
+      <c r="I76" s="18"/>
+      <c r="J76" s="18"/>
+      <c r="K76" s="18"/>
+      <c r="L76" s="18"/>
+      <c r="M76" s="18"/>
+      <c r="N76" s="18"/>
+      <c r="O76" s="18"/>
+      <c r="P76" s="18"/>
+      <c r="Q76" s="18"/>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>138</v>
+      </c>
+      <c r="C77" s="12">
+        <v>105963</v>
+      </c>
+      <c r="D77" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F77" s="18"/>
+      <c r="H77" s="18"/>
+      <c r="I77" s="18"/>
+      <c r="J77" s="18"/>
+      <c r="K77" s="18"/>
+      <c r="L77" s="18"/>
+      <c r="M77" s="18"/>
+      <c r="N77" s="18"/>
+      <c r="O77" s="18"/>
+      <c r="P77" s="18"/>
+      <c r="Q77" s="18"/>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>139</v>
+      </c>
+      <c r="C78" s="12">
+        <v>122953</v>
+      </c>
+      <c r="D78" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F78" s="18"/>
+      <c r="H78" s="18"/>
+      <c r="I78" s="18"/>
+      <c r="J78" s="18"/>
+      <c r="K78" s="18"/>
+      <c r="L78" s="18"/>
+      <c r="M78" s="18"/>
+      <c r="N78" s="18"/>
+      <c r="O78" s="18"/>
+      <c r="P78" s="18"/>
+      <c r="Q78" s="18"/>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>140</v>
+      </c>
+      <c r="C79" s="12">
+        <v>112746</v>
+      </c>
+      <c r="D79" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F79" s="18"/>
+      <c r="H79" s="18"/>
+      <c r="I79" s="18"/>
+      <c r="J79" s="18"/>
+      <c r="K79" s="18"/>
+      <c r="L79" s="18"/>
+      <c r="M79" s="18"/>
+      <c r="N79" s="18"/>
+      <c r="O79" s="18"/>
+      <c r="P79" s="18"/>
+      <c r="Q79" s="18"/>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>141</v>
+      </c>
+      <c r="C80" s="12">
+        <v>112769</v>
+      </c>
+      <c r="D80" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F80" s="18"/>
+      <c r="H80" s="18"/>
+      <c r="I80" s="18"/>
+      <c r="J80" s="18"/>
+      <c r="K80" s="18"/>
+      <c r="L80" s="18"/>
+      <c r="M80" s="18"/>
+      <c r="N80" s="18"/>
+      <c r="O80" s="18"/>
+      <c r="P80" s="18"/>
+      <c r="Q80" s="18"/>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>142</v>
+      </c>
+      <c r="C81" s="12">
+        <v>112190</v>
+      </c>
+      <c r="D81" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F81" s="18"/>
+      <c r="H81" s="18"/>
+      <c r="I81" s="18"/>
+      <c r="J81" s="18"/>
+      <c r="K81" s="18"/>
+      <c r="L81" s="18"/>
+      <c r="M81" s="18"/>
+      <c r="N81" s="18"/>
+      <c r="O81" s="18"/>
+      <c r="P81" s="18"/>
+      <c r="Q81" s="18"/>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>143</v>
+      </c>
+      <c r="C82" s="12">
+        <v>78460</v>
+      </c>
+      <c r="D82" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F82" s="18"/>
+      <c r="H82" s="18"/>
+      <c r="I82" s="18"/>
+      <c r="J82" s="18"/>
+      <c r="K82" s="18"/>
+      <c r="L82" s="18"/>
+      <c r="M82" s="18"/>
+      <c r="N82" s="18"/>
+      <c r="O82" s="18"/>
+      <c r="P82" s="18"/>
+      <c r="Q82" s="18"/>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>143</v>
+      </c>
+      <c r="C83" s="12">
+        <v>114200</v>
+      </c>
+      <c r="D83" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F83" s="18"/>
+      <c r="H83" s="18"/>
+      <c r="I83" s="18"/>
+      <c r="J83" s="18"/>
+      <c r="K83" s="18"/>
+      <c r="L83" s="18"/>
+      <c r="M83" s="18"/>
+      <c r="N83" s="18"/>
+      <c r="O83" s="18"/>
+      <c r="P83" s="18"/>
+      <c r="Q83" s="18"/>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>144</v>
+      </c>
+      <c r="C84" s="12">
+        <v>119747</v>
+      </c>
+      <c r="D84" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F84" s="18"/>
+      <c r="H84" s="18"/>
+      <c r="I84" s="18"/>
+      <c r="J84" s="18"/>
+      <c r="K84" s="18"/>
+      <c r="L84" s="18"/>
+      <c r="M84" s="18"/>
+      <c r="N84" s="18"/>
+      <c r="O84" s="18"/>
+      <c r="P84" s="18"/>
+      <c r="Q84" s="18"/>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>145</v>
+      </c>
+      <c r="C85" s="12">
+        <v>123512</v>
+      </c>
+      <c r="D85" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F85" s="18"/>
+      <c r="H85" s="18"/>
+      <c r="I85" s="18"/>
+      <c r="J85" s="18"/>
+      <c r="K85" s="18"/>
+      <c r="L85" s="18"/>
+      <c r="M85" s="18"/>
+      <c r="N85" s="18"/>
+      <c r="O85" s="18"/>
+      <c r="P85" s="18"/>
+      <c r="Q85" s="18"/>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>146</v>
+      </c>
+      <c r="C86" s="12">
+        <v>104415</v>
+      </c>
+      <c r="D86" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F86" s="18"/>
+      <c r="H86" s="18"/>
+      <c r="I86" s="18"/>
+      <c r="J86" s="18"/>
+      <c r="K86" s="18"/>
+      <c r="L86" s="18"/>
+      <c r="M86" s="18"/>
+      <c r="N86" s="18"/>
+      <c r="O86" s="18"/>
+      <c r="P86" s="18"/>
+      <c r="Q86" s="18"/>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>147</v>
+      </c>
+      <c r="C87" s="12">
+        <v>96368</v>
+      </c>
+      <c r="D87" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F87" s="18"/>
+      <c r="H87" s="18"/>
+      <c r="I87" s="18"/>
+      <c r="J87" s="18"/>
+      <c r="K87" s="18"/>
+      <c r="L87" s="18"/>
+      <c r="M87" s="18"/>
+      <c r="N87" s="18"/>
+      <c r="O87" s="18"/>
+      <c r="P87" s="18"/>
+      <c r="Q87" s="18"/>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>148</v>
+      </c>
+      <c r="C88" s="12">
+        <v>117832</v>
+      </c>
+      <c r="D88" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F88" s="18"/>
+      <c r="H88" s="18"/>
+      <c r="I88" s="18"/>
+      <c r="J88" s="18"/>
+      <c r="K88" s="18"/>
+      <c r="L88" s="18"/>
+      <c r="M88" s="18"/>
+      <c r="N88" s="18"/>
+      <c r="O88" s="18"/>
+      <c r="P88" s="18"/>
+      <c r="Q88" s="18"/>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>149</v>
+      </c>
+      <c r="C89" s="12">
+        <v>111537</v>
+      </c>
+      <c r="D89" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F89" s="18"/>
+      <c r="H89" s="18"/>
+      <c r="I89" s="18"/>
+      <c r="J89" s="18"/>
+      <c r="K89" s="18"/>
+      <c r="L89" s="18"/>
+      <c r="M89" s="18"/>
+      <c r="N89" s="18"/>
+      <c r="O89" s="18"/>
+      <c r="P89" s="18"/>
+      <c r="Q89" s="18"/>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>150</v>
+      </c>
+      <c r="C90" s="12">
+        <v>112859</v>
+      </c>
+      <c r="D90" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F90" s="18"/>
+      <c r="H90" s="18"/>
+      <c r="I90" s="18"/>
+      <c r="J90" s="18"/>
+      <c r="K90" s="18"/>
+      <c r="L90" s="18"/>
+      <c r="M90" s="18"/>
+      <c r="N90" s="18"/>
+      <c r="O90" s="18"/>
+      <c r="P90" s="18"/>
+      <c r="Q90" s="18"/>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>151</v>
+      </c>
+      <c r="C91" s="12">
+        <v>122516</v>
+      </c>
+      <c r="D91" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F91" s="18"/>
+      <c r="H91" s="18"/>
+      <c r="I91" s="18"/>
+      <c r="J91" s="18"/>
+      <c r="K91" s="18"/>
+      <c r="L91" s="18"/>
+      <c r="M91" s="18"/>
+      <c r="N91" s="18"/>
+      <c r="O91" s="18"/>
+      <c r="P91" s="18"/>
+      <c r="Q91" s="18"/>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>152</v>
+      </c>
+      <c r="C92" s="12">
+        <v>120047</v>
+      </c>
+      <c r="D92" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F92" s="18"/>
+      <c r="H92" s="18"/>
+      <c r="I92" s="18"/>
+      <c r="J92" s="18"/>
+      <c r="K92" s="18"/>
+      <c r="L92" s="18"/>
+      <c r="M92" s="18"/>
+      <c r="N92" s="18"/>
+      <c r="O92" s="18"/>
+      <c r="P92" s="18"/>
+      <c r="Q92" s="18"/>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>153</v>
+      </c>
+      <c r="C93" s="12">
+        <v>124154</v>
+      </c>
+      <c r="D93" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F93" s="18"/>
+      <c r="H93" s="18"/>
+      <c r="I93" s="18"/>
+      <c r="J93" s="18"/>
+      <c r="K93" s="18"/>
+      <c r="L93" s="18"/>
+      <c r="M93" s="18"/>
+      <c r="N93" s="18"/>
+      <c r="O93" s="18"/>
+      <c r="P93" s="18"/>
+      <c r="Q93" s="18"/>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>154</v>
+      </c>
+      <c r="C94" s="12">
+        <v>96327</v>
+      </c>
+      <c r="D94" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F94" s="18"/>
+      <c r="H94" s="18"/>
+      <c r="I94" s="18"/>
+      <c r="J94" s="18"/>
+      <c r="K94" s="18"/>
+      <c r="L94" s="18"/>
+      <c r="M94" s="18"/>
+      <c r="N94" s="18"/>
+      <c r="O94" s="18"/>
+      <c r="P94" s="18"/>
+      <c r="Q94" s="18"/>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>155</v>
+      </c>
+      <c r="C95" s="12">
+        <v>108206</v>
+      </c>
+      <c r="D95" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F95" s="18"/>
+      <c r="H95" s="18"/>
+      <c r="I95" s="18"/>
+      <c r="J95" s="18"/>
+      <c r="K95" s="18"/>
+      <c r="L95" s="18"/>
+      <c r="M95" s="18"/>
+      <c r="N95" s="18"/>
+      <c r="O95" s="18"/>
+      <c r="P95" s="18"/>
+      <c r="Q95" s="18"/>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>155</v>
+      </c>
+      <c r="C96" s="12">
+        <v>108207</v>
+      </c>
+      <c r="D96" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F96" s="18"/>
+      <c r="H96" s="18"/>
+      <c r="I96" s="18"/>
+      <c r="J96" s="18"/>
+      <c r="K96" s="18"/>
+      <c r="L96" s="18"/>
+      <c r="M96" s="18"/>
+      <c r="N96" s="18"/>
+      <c r="O96" s="18"/>
+      <c r="P96" s="18"/>
+      <c r="Q96" s="18"/>
+    </row>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>155</v>
+      </c>
+      <c r="C97" s="12">
+        <v>108208</v>
+      </c>
+      <c r="D97" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F97" s="18"/>
+      <c r="H97" s="18"/>
+      <c r="I97" s="18"/>
+      <c r="J97" s="18"/>
+      <c r="K97" s="18"/>
+      <c r="L97" s="18"/>
+      <c r="M97" s="18"/>
+      <c r="N97" s="18"/>
+      <c r="O97" s="18"/>
+      <c r="P97" s="18"/>
+      <c r="Q97" s="18"/>
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>156</v>
+      </c>
+      <c r="C98" s="12">
+        <v>123589</v>
+      </c>
+      <c r="D98" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F98" s="18"/>
+      <c r="H98" s="18"/>
+      <c r="I98" s="18"/>
+      <c r="J98" s="18"/>
+      <c r="K98" s="18"/>
+      <c r="L98" s="18"/>
+      <c r="M98" s="18"/>
+      <c r="N98" s="18"/>
+      <c r="O98" s="18"/>
+      <c r="P98" s="18"/>
+      <c r="Q98" s="18"/>
+    </row>
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>157</v>
+      </c>
+      <c r="C99" s="12">
+        <v>117346</v>
+      </c>
+      <c r="D99" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F99" s="18"/>
+      <c r="H99" s="18"/>
+      <c r="I99" s="18"/>
+      <c r="J99" s="18"/>
+      <c r="K99" s="18"/>
+      <c r="L99" s="18"/>
+      <c r="M99" s="18"/>
+      <c r="N99" s="18"/>
+      <c r="O99" s="18"/>
+      <c r="P99" s="18"/>
+      <c r="Q99" s="18"/>
+    </row>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>158</v>
+      </c>
+      <c r="C100" s="12">
+        <v>117827</v>
+      </c>
+      <c r="D100" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F100" s="18"/>
+      <c r="H100" s="18"/>
+      <c r="I100" s="18"/>
+      <c r="J100" s="18"/>
+      <c r="K100" s="18"/>
+      <c r="L100" s="18"/>
+      <c r="M100" s="18"/>
+      <c r="N100" s="18"/>
+      <c r="O100" s="18"/>
+      <c r="P100" s="18"/>
+      <c r="Q100" s="18"/>
+    </row>
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>159</v>
+      </c>
+      <c r="C101" s="12">
+        <v>120427</v>
+      </c>
+      <c r="D101" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F101" s="18"/>
+      <c r="H101" s="18"/>
+      <c r="I101" s="18"/>
+      <c r="J101" s="18"/>
+      <c r="K101" s="18"/>
+      <c r="L101" s="18"/>
+      <c r="M101" s="18"/>
+      <c r="N101" s="18"/>
+      <c r="O101" s="18"/>
+      <c r="P101" s="18"/>
+      <c r="Q101" s="18"/>
+    </row>
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>160</v>
+      </c>
+      <c r="C102" s="12">
+        <v>117190</v>
+      </c>
+      <c r="D102" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F102" s="18"/>
+      <c r="H102" s="18"/>
+      <c r="I102" s="18"/>
+      <c r="J102" s="18"/>
+      <c r="K102" s="18"/>
+      <c r="L102" s="18"/>
+      <c r="M102" s="18"/>
+      <c r="N102" s="18"/>
+      <c r="O102" s="18"/>
+      <c r="P102" s="18"/>
+      <c r="Q102" s="18"/>
+    </row>
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>161</v>
+      </c>
+      <c r="C103" s="12">
+        <v>105580</v>
+      </c>
+      <c r="D103" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F103" s="18"/>
+      <c r="H103" s="18"/>
+      <c r="I103" s="18"/>
+      <c r="J103" s="18"/>
+      <c r="K103" s="18"/>
+      <c r="L103" s="18"/>
+      <c r="M103" s="18"/>
+      <c r="N103" s="18"/>
+      <c r="O103" s="18"/>
+      <c r="P103" s="18"/>
+      <c r="Q103" s="18"/>
+    </row>
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>162</v>
+      </c>
+      <c r="C104" s="12">
+        <v>120355</v>
+      </c>
+      <c r="D104" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F104" s="18"/>
+      <c r="H104" s="18"/>
+      <c r="I104" s="18"/>
+      <c r="J104" s="18"/>
+      <c r="K104" s="18"/>
+      <c r="L104" s="18"/>
+      <c r="M104" s="18"/>
+      <c r="N104" s="18"/>
+      <c r="O104" s="18"/>
+      <c r="P104" s="18"/>
+      <c r="Q104" s="18"/>
+    </row>
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>163</v>
+      </c>
+      <c r="C105" s="12">
+        <v>116594</v>
+      </c>
+      <c r="D105" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F105" s="18"/>
+      <c r="H105" s="18"/>
+      <c r="I105" s="18"/>
+      <c r="J105" s="18"/>
+      <c r="K105" s="18"/>
+      <c r="L105" s="18"/>
+      <c r="M105" s="18"/>
+      <c r="N105" s="18"/>
+      <c r="O105" s="18"/>
+      <c r="P105" s="18"/>
+      <c r="Q105" s="18"/>
+    </row>
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>164</v>
+      </c>
+      <c r="C106" s="12">
+        <v>125640</v>
+      </c>
+      <c r="D106" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F106" s="18"/>
+      <c r="H106" s="18"/>
+      <c r="I106" s="18"/>
+      <c r="J106" s="18"/>
+      <c r="K106" s="18"/>
+      <c r="L106" s="18"/>
+      <c r="M106" s="18"/>
+      <c r="N106" s="18"/>
+      <c r="O106" s="18"/>
+      <c r="P106" s="18"/>
+      <c r="Q106" s="18"/>
+    </row>
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>165</v>
+      </c>
+      <c r="C107" s="12">
+        <v>107967</v>
+      </c>
+      <c r="D107" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F107" s="18"/>
+      <c r="H107" s="18"/>
+      <c r="I107" s="18"/>
+      <c r="J107" s="18"/>
+      <c r="K107" s="18"/>
+      <c r="L107" s="18"/>
+      <c r="M107" s="18"/>
+      <c r="N107" s="18"/>
+      <c r="O107" s="18"/>
+      <c r="P107" s="18"/>
+      <c r="Q107" s="18"/>
+    </row>
+    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>166</v>
+      </c>
+      <c r="C108" s="12">
+        <v>3913</v>
+      </c>
+      <c r="D108" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F108" s="18"/>
+      <c r="H108" s="18"/>
+      <c r="I108" s="18"/>
+      <c r="J108" s="18"/>
+      <c r="K108" s="18"/>
+      <c r="L108" s="18"/>
+      <c r="M108" s="18"/>
+      <c r="N108" s="18"/>
+      <c r="O108" s="18"/>
+      <c r="P108" s="18"/>
+      <c r="Q108" s="18"/>
+    </row>
+    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>167</v>
+      </c>
+      <c r="C109" s="12">
+        <v>115211</v>
+      </c>
+      <c r="D109" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F109" s="18"/>
+      <c r="H109" s="18"/>
+      <c r="I109" s="18"/>
+      <c r="J109" s="18"/>
+      <c r="K109" s="18"/>
+      <c r="L109" s="18"/>
+      <c r="M109" s="18"/>
+      <c r="N109" s="18"/>
+      <c r="O109" s="18"/>
+      <c r="P109" s="18"/>
+      <c r="Q109" s="18"/>
+    </row>
+    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>168</v>
+      </c>
+      <c r="C110" s="12">
+        <v>96132</v>
+      </c>
+      <c r="D110" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F110" s="18"/>
+      <c r="H110" s="18"/>
+      <c r="I110" s="18"/>
+      <c r="J110" s="18"/>
+      <c r="K110" s="18"/>
+      <c r="L110" s="18"/>
+      <c r="M110" s="18"/>
+      <c r="N110" s="18"/>
+      <c r="O110" s="18"/>
+      <c r="P110" s="18"/>
+      <c r="Q110" s="18"/>
+    </row>
+    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>169</v>
+      </c>
+      <c r="C111" s="12">
+        <v>113779</v>
+      </c>
+      <c r="D111" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F111" s="18"/>
+      <c r="H111" s="18"/>
+      <c r="I111" s="18"/>
+      <c r="J111" s="18"/>
+      <c r="K111" s="18"/>
+      <c r="L111" s="18"/>
+      <c r="M111" s="18"/>
+      <c r="N111" s="18"/>
+      <c r="O111" s="18"/>
+      <c r="P111" s="18"/>
+      <c r="Q111" s="18"/>
+    </row>
+    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>170</v>
+      </c>
+      <c r="C112" s="12">
+        <v>96002</v>
+      </c>
+      <c r="D112" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F112" s="18"/>
+      <c r="H112" s="18"/>
+      <c r="I112" s="18"/>
+      <c r="J112" s="18"/>
+      <c r="K112" s="18"/>
+      <c r="L112" s="18"/>
+      <c r="M112" s="18"/>
+      <c r="N112" s="18"/>
+      <c r="O112" s="18"/>
+      <c r="P112" s="18"/>
+      <c r="Q112" s="18"/>
+    </row>
+    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>171</v>
+      </c>
+      <c r="C113" s="12">
+        <v>120523</v>
+      </c>
+      <c r="D113" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F113" s="18"/>
+      <c r="H113" s="18"/>
+      <c r="I113" s="18"/>
+      <c r="J113" s="18"/>
+      <c r="K113" s="18"/>
+      <c r="L113" s="18"/>
+      <c r="M113" s="18"/>
+      <c r="N113" s="18"/>
+      <c r="O113" s="18"/>
+      <c r="P113" s="18"/>
+      <c r="Q113" s="18"/>
+    </row>
+    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>172</v>
+      </c>
+      <c r="C114" s="12">
+        <v>120882</v>
+      </c>
+      <c r="D114" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F114" s="18"/>
+      <c r="H114" s="18"/>
+      <c r="I114" s="18"/>
+      <c r="J114" s="18"/>
+      <c r="K114" s="18"/>
+      <c r="L114" s="18"/>
+      <c r="M114" s="18"/>
+      <c r="N114" s="18"/>
+      <c r="O114" s="18"/>
+      <c r="P114" s="18"/>
+      <c r="Q114" s="18"/>
+    </row>
+    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>173</v>
+      </c>
+      <c r="C115" s="12">
+        <v>120884</v>
+      </c>
+      <c r="D115" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F115" s="18"/>
+      <c r="H115" s="18"/>
+      <c r="I115" s="18"/>
+      <c r="J115" s="18"/>
+      <c r="K115" s="18"/>
+      <c r="L115" s="18"/>
+      <c r="M115" s="18"/>
+      <c r="N115" s="18"/>
+      <c r="O115" s="18"/>
+      <c r="P115" s="18"/>
+      <c r="Q115" s="18"/>
+    </row>
+    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>174</v>
+      </c>
+      <c r="C116" s="12">
+        <v>120880</v>
+      </c>
+      <c r="D116" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="F116" s="18"/>
+      <c r="H116" s="18"/>
+      <c r="I116" s="18"/>
+      <c r="J116" s="18"/>
+      <c r="K116" s="18"/>
+      <c r="L116" s="18"/>
+      <c r="M116" s="18"/>
+      <c r="N116" s="18"/>
+      <c r="O116" s="18"/>
+      <c r="P116" s="18"/>
+      <c r="Q116" s="18"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:Q116 F2:F116" xr:uid="{DD647EC7-AA3B-456C-B526-D2C7566DD6E9}">
+      <formula1>"Keep, Delete, Modify, Merge, TBD"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C2CA369-FD74-45DA-B52B-B2E81C788AE9}">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -950,7 +4524,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40C63F19-829C-498F-95B9-00BAFFFCE5E2}">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -1036,7 +4610,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EED0CC8C-2B0B-4197-BECD-51476140892C}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1098,11 +4672,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD17310C-D201-4D02-99D2-460358C605A4}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>